<commit_message>
fixed defect number 1
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R40" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R49" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="R58" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="R66" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="R78" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="R89" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="R97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="R106" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R115" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R124" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="R133" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="R142" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
block.py now makes sense :)
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="R3" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="R17" t="n">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="R23" t="n">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="R32" t="n">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="R40" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="R49" t="n">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="R58" t="n">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="R66" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="R74" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="R78" t="n">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="R89" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="R97" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="R106" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="R115" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="R124" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="R133" t="n">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="R142" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
saving my changes before my pc dies
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="R3" t="n">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="R17" t="n">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="R23" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="R32" t="n">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
+        <v>18</v>
+      </c>
+      <c r="R40" t="n">
         <v>15</v>
-      </c>
-      <c r="R40" t="n">
-        <v>7</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R49" t="n">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R58" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,7 +4379,7 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="R66" t="n">
         <v>8</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="R74" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="R78" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="R89" t="n">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="R97" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="R106" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="R115" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="R124" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="R133" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="R142" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updates to time module
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="R3" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="R10" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="R17" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="R23" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="R32" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="R40" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="R49" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="R58" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="R66" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="R74" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="R78" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="R89" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="R97" t="n">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="R106" t="n">
         <v>22</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="R115" t="n">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R124" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="R133" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="R142" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
commented out HW UI update
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="R3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="R17" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="R23" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="R32" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="R40" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R49" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="R58" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="R66" t="n">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="R74" t="n">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="R78" t="n">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="R89" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="R97" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6694,7 +6694,7 @@
         <v>46</v>
       </c>
       <c r="R106" t="n">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="R115" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="R124" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="R133" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="R142" t="n">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
debugging, just adding comments
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="R3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R10" t="n">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="R17" t="n">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="R23" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="R32" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="R40" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="R49" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="R58" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="R66" t="n">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="R74" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="R78" t="n">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="R89" t="n">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="R97" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="R106" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="R115" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="R124" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="R133" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8824,7 +8824,7 @@
         <v>70</v>
       </c>
       <c r="R142" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
5:40PM UI going smooth
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="R3" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="R10" t="n">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="R23" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="R32" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="R40" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="R49" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="R58" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="R66" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="R74" t="n">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="R78" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="R89" t="n">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="R97" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="R106" t="n">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="R115" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="R124" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="R133" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="R142" t="n">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
trouble shooting track controller
</commit_message>
<xml_diff>
--- a/testing_output.xlsx
+++ b/testing_output.xlsx
@@ -651,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="R3" t="n">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="R10" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="R17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1829,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="R23" t="n">
         <v>3</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="R32" t="n">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="R40" t="n">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -3369,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="R49" t="n">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -3915,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="R58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4379,10 +4379,10 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="R66" t="n">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="R74" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="R78" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -5713,10 +5713,10 @@
         <v>0</v>
       </c>
       <c r="Q89" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="R89" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
@@ -6173,10 +6173,10 @@
         <v>0</v>
       </c>
       <c r="Q97" t="n">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="R97" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="S97" t="n">
         <v>0</v>
@@ -6691,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="Q106" t="n">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="R106" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="S106" t="n">
         <v>0</v>
@@ -7211,10 +7211,10 @@
         <v>0</v>
       </c>
       <c r="Q115" t="n">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="R115" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="S115" t="n">
         <v>0</v>
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="Q124" t="n">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="R124" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S124" t="n">
         <v>0</v>
@@ -8275,10 +8275,10 @@
         <v>0</v>
       </c>
       <c r="Q133" t="n">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="R133" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -8821,10 +8821,10 @@
         <v>0</v>
       </c>
       <c r="Q142" t="n">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="R142" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="S142" t="n">
         <v>0</v>

</xml_diff>